<commit_message>
현재 이름, 생년월일, 주소, 휴대폰번호, 프로필사진 보기 쿼리문 수정; getUserInfo: birth -> to_char(birth, 'yyyy/mm/dd')
</commit_message>
<xml_diff>
--- a/Matrix진행현황관리.xlsx
+++ b/Matrix진행현황관리.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DACDBF3B-AA1B-4F59-AF78-3869D84932BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0753C2C3-DB0D-42D7-9A16-0980B165AE1A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1946,10 +1946,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select name, birth, email, address_city||' '||address_gu||' '||address_dong as address, phone_num, profile_photo from users where user_id=? ;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회원탈퇴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1972,6 +1968,10 @@
 and u.user_id=a.admin_id
 and a.branch_seq=b.branch_seq
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">select name, to_char(birth, 'yyyy/mm/dd'), email, address_city||' '||address_gu||' '||address_dong as address, phone_num, profile_photo from users where user_id=? </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5423,8 +5423,8 @@
   <sheetPr codeName="Sheet6" filterMode="1"/>
   <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126:F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6683,12 +6683,12 @@
       </c>
       <c r="B107" s="100"/>
       <c r="C107" s="83" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D107" s="84"/>
       <c r="E107" s="85"/>
       <c r="F107" s="82" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="108" spans="1:6" hidden="1">
@@ -6906,7 +6906,7 @@
         <v>144</v>
       </c>
       <c r="F126" s="82" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="127" spans="1:6" hidden="1">
@@ -7240,7 +7240,7 @@
       </c>
       <c r="E159" s="85"/>
       <c r="F159" s="86" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="160" spans="1:6" hidden="1">

</xml_diff>

<commit_message>
StaffDAO, staffMapper 구현. mybatis설정파일 수정. Test 코드 추가.
</commit_message>
<xml_diff>
--- a/Matrix진행현황관리.xlsx
+++ b/Matrix진행현황관리.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D55F5D4D-D229-432A-8713-457C39E493E0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="진행일정" sheetId="3" r:id="rId1"/>
@@ -20,9 +19,9 @@
     <sheet name="발표컨텐츠" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SQL!$F$1:$F$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SQL!$B$1:$B$163</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1982,7 +1981,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-412]m&quot;월&quot;\ d&quot;일&quot;\ dddd"/>
   </numFmts>
@@ -2604,7 +2603,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="표준 2" xfId="1"/>
     <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2923,7 +2922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H48"/>
   <sheetViews>
@@ -2932,19 +2931,19 @@
       <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="36"/>
-    <col min="2" max="2" width="16.125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="31.125" customWidth="1"/>
-    <col min="4" max="4" width="31.25" customWidth="1"/>
-    <col min="5" max="5" width="34.75" customWidth="1"/>
+    <col min="1" max="1" width="8.69921875" style="36"/>
+    <col min="2" max="2" width="16.09765625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="31.09765625" customWidth="1"/>
+    <col min="4" max="4" width="31.19921875" customWidth="1"/>
+    <col min="5" max="5" width="34.69921875" customWidth="1"/>
     <col min="6" max="6" width="31.5" customWidth="1"/>
-    <col min="7" max="7" width="34.625" customWidth="1"/>
-    <col min="8" max="8" width="31.625" customWidth="1"/>
+    <col min="7" max="7" width="34.59765625" customWidth="1"/>
+    <col min="8" max="8" width="31.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="35" t="s">
         <v>215</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B2" s="17">
         <v>43214</v>
       </c>
@@ -2978,19 +2977,19 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B3" s="17">
         <v>43215</v>
       </c>
       <c r="C3" s="15"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B4" s="17">
         <v>43216</v>
       </c>
       <c r="C4" s="15"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B5" s="17">
         <v>43217</v>
       </c>
@@ -2998,31 +2997,31 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B6" s="18">
         <v>43218</v>
       </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B7" s="18">
         <v>43219</v>
       </c>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B8" s="17">
         <v>43220</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B9" s="17">
         <v>43221</v>
       </c>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B10" s="17">
         <v>43222</v>
       </c>
@@ -3030,7 +3029,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B11" s="17">
         <v>43223</v>
       </c>
@@ -3038,7 +3037,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B12" s="17">
         <v>43224</v>
       </c>
@@ -3046,31 +3045,31 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B13" s="18">
         <v>43225</v>
       </c>
       <c r="C13" s="15"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B14" s="18">
         <v>43226</v>
       </c>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B15" s="18">
         <v>43227</v>
       </c>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B16" s="17">
         <v>43228</v>
       </c>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B17" s="33">
         <v>43229</v>
       </c>
@@ -3081,7 +3080,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.4">
       <c r="B18" s="32">
         <v>43230</v>
       </c>
@@ -3104,7 +3103,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="87" x14ac:dyDescent="0.4">
       <c r="B19" s="32">
         <v>43231</v>
       </c>
@@ -3127,19 +3126,19 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B20" s="18">
         <v>43232</v>
       </c>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B21" s="18">
         <v>43233</v>
       </c>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="B22" s="19">
         <v>43234</v>
       </c>
@@ -3162,7 +3161,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.4">
       <c r="B23" s="19">
         <v>43235</v>
       </c>
@@ -3185,7 +3184,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>381</v>
       </c>
@@ -3193,7 +3192,7 @@
         <v>43236</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="36" t="s">
         <v>209</v>
       </c>
@@ -3202,7 +3201,7 @@
       </c>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="36" t="s">
         <v>209</v>
       </c>
@@ -3211,19 +3210,19 @@
       </c>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B27" s="18">
         <v>43239</v>
       </c>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B28" s="18">
         <v>43240</v>
       </c>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="36" t="s">
         <v>210</v>
       </c>
@@ -3232,7 +3231,7 @@
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="36" t="s">
         <v>211</v>
       </c>
@@ -3241,37 +3240,37 @@
       </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B31" s="19">
         <v>43243</v>
       </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B32" s="19">
         <v>43244</v>
       </c>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B33" s="19">
         <v>43245</v>
       </c>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B34" s="18">
         <v>43246</v>
       </c>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B35" s="18">
         <v>43247</v>
       </c>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B36" s="19">
         <v>43248</v>
       </c>
@@ -3279,13 +3278,13 @@
         <v>184</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B37" s="19">
         <v>43249</v>
       </c>
       <c r="C37" s="15"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B38" s="19">
         <v>43250</v>
       </c>
@@ -3293,7 +3292,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" s="36" t="s">
         <v>209</v>
       </c>
@@ -3302,31 +3301,31 @@
       </c>
       <c r="C39" s="15"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B40" s="17">
         <v>43252</v>
       </c>
       <c r="C40" s="15"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B41" s="18">
         <v>43253</v>
       </c>
       <c r="C41" s="15"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B42" s="18">
         <v>43254</v>
       </c>
       <c r="C42" s="15"/>
     </row>
-    <row r="43" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B43" s="19">
         <v>43255</v>
       </c>
       <c r="C43" s="15"/>
     </row>
-    <row r="44" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B44" s="20">
         <v>43256</v>
       </c>
@@ -3334,19 +3333,19 @@
         <v>185</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B45" s="18">
         <v>43257</v>
       </c>
       <c r="C45" s="15"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B46" s="19">
         <v>43258</v>
       </c>
       <c r="C46" s="15"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B47" s="19">
         <v>43259</v>
       </c>
@@ -3354,7 +3353,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B48" s="17"/>
       <c r="C48" s="15"/>
     </row>
@@ -3366,7 +3365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K155"/>
   <sheetViews>
@@ -3375,22 +3374,22 @@
       <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.75" customWidth="1"/>
-    <col min="2" max="2" width="6.875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="5.375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="50.75" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.25" customWidth="1"/>
-    <col min="6" max="6" width="19.625" customWidth="1"/>
+    <col min="1" max="1" width="4.69921875" customWidth="1"/>
+    <col min="2" max="2" width="6.8984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.3984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="50.69921875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23.19921875" customWidth="1"/>
+    <col min="6" max="6" width="19.59765625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="9" max="9" width="11.625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="11.75" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.75" style="7"/>
+    <col min="9" max="9" width="11.59765625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.69921875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="8.69921875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -3421,7 +3420,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -3439,7 +3438,7 @@
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -3455,7 +3454,7 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -3479,7 +3478,7 @@
       </c>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -3503,7 +3502,7 @@
       </c>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -3519,7 +3518,7 @@
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -3535,7 +3534,7 @@
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -3551,7 +3550,7 @@
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -3567,7 +3566,7 @@
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -3583,7 +3582,7 @@
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -3609,7 +3608,7 @@
       </c>
       <c r="J11" s="28"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -3620,7 +3619,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -3636,7 +3635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -3667,7 +3666,7 @@
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
     </row>
-    <row r="16" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -3690,7 +3689,7 @@
       </c>
       <c r="J16" s="22"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -3705,7 +3704,7 @@
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -3728,7 +3727,7 @@
       </c>
       <c r="J18" s="22"/>
     </row>
-    <row r="19" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -3751,7 +3750,7 @@
       </c>
       <c r="J19" s="22"/>
     </row>
-    <row r="20" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -3774,7 +3773,7 @@
       </c>
       <c r="J20" s="22"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -3789,7 +3788,7 @@
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -3804,7 +3803,7 @@
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -3819,7 +3818,7 @@
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -3844,7 +3843,7 @@
       </c>
       <c r="J24" s="55"/>
     </row>
-    <row r="25" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -3867,7 +3866,7 @@
       </c>
       <c r="J25" s="55"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -3882,7 +3881,7 @@
       <c r="I26" s="55"/>
       <c r="J26" s="55"/>
     </row>
-    <row r="27" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -3908,7 +3907,7 @@
       </c>
       <c r="J27" s="28"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -3924,7 +3923,7 @@
       <c r="I28" s="28"/>
       <c r="J28" s="28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -3940,7 +3939,7 @@
       <c r="I29" s="57"/>
       <c r="J29" s="57"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -3958,7 +3957,7 @@
       <c r="I30" s="57"/>
       <c r="J30" s="57"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -3976,7 +3975,7 @@
       <c r="I31" s="57"/>
       <c r="J31" s="57"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -3992,7 +3991,7 @@
       <c r="I32" s="28"/>
       <c r="J32" s="28"/>
     </row>
-    <row r="33" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A33" s="14">
         <v>32</v>
       </c>
@@ -4016,7 +4015,7 @@
       </c>
       <c r="J33" s="28"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="14">
         <v>33</v>
       </c>
@@ -4032,7 +4031,7 @@
       <c r="I34" s="28"/>
       <c r="J34" s="28"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -4056,7 +4055,7 @@
       </c>
       <c r="J35" s="28"/>
     </row>
-    <row r="36" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A36" s="14">
         <v>35</v>
       </c>
@@ -4080,7 +4079,7 @@
       </c>
       <c r="J36" s="28"/>
     </row>
-    <row r="37" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A37" s="14">
         <v>36</v>
       </c>
@@ -4104,7 +4103,7 @@
       </c>
       <c r="J37" s="28"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="14">
         <v>37</v>
       </c>
@@ -4120,7 +4119,7 @@
       <c r="I38" s="28"/>
       <c r="J38" s="28"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="14">
         <v>38</v>
       </c>
@@ -4136,7 +4135,7 @@
       <c r="I39" s="28"/>
       <c r="J39" s="28"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="14">
         <v>39</v>
       </c>
@@ -4152,7 +4151,7 @@
       <c r="I40" s="28"/>
       <c r="J40" s="28"/>
     </row>
-    <row r="41" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A41" s="14">
         <v>40</v>
       </c>
@@ -4178,7 +4177,7 @@
       </c>
       <c r="J41" s="28"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="14">
         <v>41</v>
       </c>
@@ -4202,7 +4201,7 @@
       </c>
       <c r="J42" s="55"/>
     </row>
-    <row r="43" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A43" s="14">
         <v>42</v>
       </c>
@@ -4226,7 +4225,7 @@
       </c>
       <c r="J43" s="55"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="14">
         <v>43</v>
       </c>
@@ -4242,7 +4241,7 @@
       <c r="I44" s="28"/>
       <c r="J44" s="28"/>
     </row>
-    <row r="45" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A45" s="14">
         <v>44</v>
       </c>
@@ -4268,7 +4267,7 @@
       </c>
       <c r="J45" s="28"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="14">
         <v>45</v>
       </c>
@@ -4284,7 +4283,7 @@
       <c r="I46" s="28"/>
       <c r="J46" s="28"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="14">
         <v>46</v>
       </c>
@@ -4302,7 +4301,7 @@
       <c r="I47" s="22"/>
       <c r="J47" s="22"/>
     </row>
-    <row r="48" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A48" s="14">
         <v>47</v>
       </c>
@@ -4326,7 +4325,7 @@
       </c>
       <c r="J48" s="22"/>
     </row>
-    <row r="49" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A49" s="14">
         <v>48</v>
       </c>
@@ -4350,7 +4349,7 @@
       </c>
       <c r="J49" s="22"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4361,7 +4360,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4375,7 +4374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4386,7 +4385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4397,7 +4396,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4411,7 +4410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4422,7 +4421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4436,7 +4435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4450,7 +4449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4467,7 +4466,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4475,7 +4474,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4483,7 +4482,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4494,7 +4493,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4505,7 +4504,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4519,7 +4518,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4527,7 +4526,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4538,7 +4537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4546,7 +4545,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4554,7 +4553,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4568,7 +4567,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4579,7 +4578,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4587,7 +4586,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4598,7 +4597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4606,7 +4605,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4614,7 +4613,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4622,7 +4621,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4630,7 +4629,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4638,7 +4637,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4646,7 +4645,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4654,7 +4653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4662,7 +4661,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4670,7 +4669,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4678,7 +4677,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4697,7 +4696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4708,7 +4707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4716,7 +4715,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4724,7 +4723,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4732,7 +4731,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4740,7 +4739,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4762,7 +4761,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4770,7 +4769,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4792,7 +4791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4800,7 +4799,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4808,7 +4807,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4816,7 +4815,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4827,7 +4826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4841,7 +4840,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4849,7 +4848,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4857,7 +4856,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4868,7 +4867,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4882,7 +4881,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4890,7 +4889,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4901,7 +4900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4912,7 +4911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4926,7 +4925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4940,7 +4939,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4962,7 +4961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4973,7 +4972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4984,7 +4983,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4992,7 +4991,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5000,7 +4999,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5019,7 +5018,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5030,7 +5029,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5041,7 +5040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5055,7 +5054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5079,7 +5078,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5087,7 +5086,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5103,7 +5102,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5111,7 +5110,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5119,7 +5118,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5127,7 +5126,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5138,7 +5137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5146,7 +5145,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5157,7 +5156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5168,7 +5167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5176,7 +5175,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5184,7 +5183,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5198,7 +5197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5209,7 +5208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5217,7 +5216,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5225,7 +5224,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5233,7 +5232,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5241,7 +5240,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5249,7 +5248,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5257,7 +5256,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5271,7 +5270,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5282,7 +5281,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5290,7 +5289,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5298,7 +5297,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5306,7 +5305,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5314,7 +5313,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5322,7 +5321,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5333,7 +5332,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5344,7 +5343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5355,7 +5354,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5372,7 +5371,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5386,7 +5385,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5397,7 +5396,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.4">
       <c r="H155">
         <f>COUNTA(H2:H154)</f>
         <v>61</v>
@@ -5414,26 +5413,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.75" customWidth="1"/>
-    <col min="2" max="2" width="10.25" style="47" customWidth="1"/>
-    <col min="3" max="3" width="6.75" style="70" customWidth="1"/>
-    <col min="4" max="4" width="5.25" style="75" customWidth="1"/>
+    <col min="1" max="1" width="4.69921875" customWidth="1"/>
+    <col min="2" max="2" width="10.19921875" style="47" customWidth="1"/>
+    <col min="3" max="3" width="6.69921875" style="70" customWidth="1"/>
+    <col min="4" max="4" width="5.19921875" style="75" customWidth="1"/>
     <col min="5" max="5" width="62.5" style="64" customWidth="1"/>
     <col min="6" max="6" width="179" customWidth="1"/>
     <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="58" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="58" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="58" t="s">
         <v>288</v>
       </c>
@@ -5452,7 +5451,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -5464,7 +5463,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -5477,7 +5476,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -5496,7 +5495,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -5515,7 +5514,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -5526,7 +5525,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -5537,7 +5536,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -5548,7 +5547,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -5559,7 +5558,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -5567,7 +5566,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="109.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="109.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -5583,7 +5582,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -5591,7 +5590,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -5605,7 +5604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -5619,7 +5618,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -5631,7 +5630,7 @@
       <c r="E15" s="66"/>
       <c r="F15" s="43"/>
     </row>
-    <row r="16" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -5647,7 +5646,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -5659,7 +5658,7 @@
       <c r="E17" s="66"/>
       <c r="F17" s="43"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -5675,7 +5674,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -5691,7 +5690,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -5707,7 +5706,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -5723,7 +5722,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -5731,7 +5730,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -5747,7 +5746,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -5763,7 +5762,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -5771,7 +5770,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="165" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="174" x14ac:dyDescent="0.4">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -5787,7 +5786,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -5796,7 +5795,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -5804,7 +5803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -5815,7 +5814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -5826,7 +5825,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -5838,7 +5837,7 @@
       <c r="E32" s="66"/>
       <c r="F32" s="43"/>
     </row>
-    <row r="33" spans="1:6" ht="66" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A33" s="14">
         <v>32</v>
       </c>
@@ -5854,7 +5853,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="14">
         <v>33</v>
       </c>
@@ -5862,7 +5861,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -5878,7 +5877,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A36" s="14">
         <v>35</v>
       </c>
@@ -5894,7 +5893,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A37" s="14">
         <v>36</v>
       </c>
@@ -5910,7 +5909,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" s="14">
         <v>37</v>
       </c>
@@ -5918,7 +5917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" s="14">
         <v>38</v>
       </c>
@@ -5932,7 +5931,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" s="14">
         <v>39</v>
       </c>
@@ -5940,7 +5939,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" s="14">
         <v>40</v>
       </c>
@@ -5956,7 +5955,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" s="14">
         <v>41</v>
       </c>
@@ -5972,7 +5971,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" s="14">
         <v>42</v>
       </c>
@@ -5988,7 +5987,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" s="14">
         <v>43</v>
       </c>
@@ -5996,7 +5995,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" s="14">
         <v>44</v>
       </c>
@@ -6012,7 +6011,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" s="14">
         <v>45</v>
       </c>
@@ -6020,7 +6019,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" s="14">
         <v>46</v>
       </c>
@@ -6032,7 +6031,7 @@
       <c r="E47" s="66"/>
       <c r="F47" s="43"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" s="14">
         <v>47</v>
       </c>
@@ -6044,7 +6043,7 @@
       <c r="E48" s="66"/>
       <c r="F48" s="49"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" s="14">
         <v>48</v>
       </c>
@@ -6060,7 +6059,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A50" s="14">
         <v>49</v>
       </c>
@@ -6076,7 +6075,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A51" s="14">
         <v>50</v>
       </c>
@@ -6092,7 +6091,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" s="14">
         <v>51</v>
       </c>
@@ -6104,7 +6103,7 @@
       <c r="E52" s="66"/>
       <c r="F52" s="49"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" s="14">
         <v>52</v>
       </c>
@@ -6120,7 +6119,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A54" s="14">
         <v>53</v>
       </c>
@@ -6136,7 +6135,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A55" s="14">
         <v>54</v>
       </c>
@@ -6152,7 +6151,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A56" s="43">
         <v>55</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57" s="43">
         <v>56</v>
       </c>
@@ -6180,7 +6179,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58" s="43">
         <v>57</v>
       </c>
@@ -6194,7 +6193,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A59" s="43">
         <v>58</v>
       </c>
@@ -6208,7 +6207,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A60" s="43">
         <v>59</v>
       </c>
@@ -6222,7 +6221,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61" s="43">
         <v>60</v>
       </c>
@@ -6236,7 +6235,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A62" s="43">
         <v>61</v>
       </c>
@@ -6250,7 +6249,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63" s="43">
         <v>62</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64" s="43">
         <v>63</v>
       </c>
@@ -6278,7 +6277,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A65" s="43">
         <v>64</v>
       </c>
@@ -6286,7 +6285,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A66" s="43">
         <v>65</v>
       </c>
@@ -6294,7 +6293,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A67" s="43">
         <v>66</v>
       </c>
@@ -6308,7 +6307,7 @@
       <c r="E67" s="66"/>
       <c r="F67" s="43"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68" s="43">
         <v>67</v>
       </c>
@@ -6316,7 +6315,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A69" s="43">
         <v>68</v>
       </c>
@@ -6330,7 +6329,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A70" s="43">
         <v>69</v>
       </c>
@@ -6338,7 +6337,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A71" s="43">
         <v>70</v>
       </c>
@@ -6352,7 +6351,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A72" s="43">
         <v>71</v>
       </c>
@@ -6360,7 +6359,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A73" s="43">
         <v>72</v>
       </c>
@@ -6368,7 +6367,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A74" s="43">
         <v>73</v>
       </c>
@@ -6379,7 +6378,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A75" s="43">
         <v>74</v>
       </c>
@@ -6387,7 +6386,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A76" s="43">
         <v>75</v>
       </c>
@@ -6395,7 +6394,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A77" s="43">
         <v>76</v>
       </c>
@@ -6409,7 +6408,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A78" s="43">
         <v>77</v>
       </c>
@@ -6417,7 +6416,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A79" s="43">
         <v>78</v>
       </c>
@@ -6425,7 +6424,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A80" s="43">
         <v>79</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A81" s="43">
         <v>80</v>
       </c>
@@ -6441,7 +6440,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A82" s="43">
         <v>81</v>
       </c>
@@ -6449,7 +6448,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A83" s="43">
         <v>82</v>
       </c>
@@ -6457,7 +6456,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A84" s="43">
         <v>83</v>
       </c>
@@ -6465,7 +6464,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A85" s="43">
         <v>84</v>
       </c>
@@ -6473,7 +6472,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A86" s="43">
         <v>85</v>
       </c>
@@ -6481,7 +6480,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A87" s="43">
         <v>86</v>
       </c>
@@ -6489,7 +6488,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A88" s="43">
         <v>87</v>
       </c>
@@ -6497,7 +6496,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A89" s="43">
         <v>88</v>
       </c>
@@ -6505,7 +6504,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A90" s="43">
         <v>89</v>
       </c>
@@ -6514,7 +6513,7 @@
       </c>
       <c r="F90" s="64"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A91" s="43">
         <v>90</v>
       </c>
@@ -6522,7 +6521,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A92" s="43">
         <v>91</v>
       </c>
@@ -6538,7 +6537,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A93" s="43">
         <v>92</v>
       </c>
@@ -6547,7 +6546,7 @@
       </c>
       <c r="F93" s="64"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A94" s="43">
         <v>93</v>
       </c>
@@ -6555,7 +6554,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A95" s="43">
         <v>94</v>
       </c>
@@ -6566,7 +6565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A96" s="43">
         <v>95</v>
       </c>
@@ -6580,7 +6579,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A97" s="43">
         <v>96</v>
       </c>
@@ -6588,7 +6587,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A98" s="43">
         <v>97</v>
       </c>
@@ -6602,7 +6601,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A99" s="43">
         <v>98</v>
       </c>
@@ -6616,7 +6615,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A100" s="43">
         <v>99</v>
       </c>
@@ -6624,7 +6623,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A101" s="43">
         <v>100</v>
       </c>
@@ -6632,7 +6631,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A102" s="43">
         <v>101</v>
       </c>
@@ -6640,7 +6639,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A103" s="43">
         <v>102</v>
       </c>
@@ -6651,7 +6650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A104" s="43">
         <v>103</v>
       </c>
@@ -6662,7 +6661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A105" s="43">
         <v>104</v>
       </c>
@@ -6670,7 +6669,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A106" s="43">
         <v>105</v>
       </c>
@@ -6678,7 +6677,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A107" s="43">
         <v>106</v>
       </c>
@@ -6692,7 +6691,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A108" s="43">
         <v>107</v>
       </c>
@@ -6700,7 +6699,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A109" s="43">
         <v>108</v>
       </c>
@@ -6714,7 +6713,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A110" s="43">
         <v>109</v>
       </c>
@@ -6722,7 +6721,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A111" s="43">
         <v>110</v>
       </c>
@@ -6736,7 +6735,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A112" s="43">
         <v>111</v>
       </c>
@@ -6750,7 +6749,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="231" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="243.6" x14ac:dyDescent="0.4">
       <c r="A113" s="43">
         <v>112</v>
       </c>
@@ -6764,7 +6763,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A114" s="43">
         <v>113</v>
       </c>
@@ -6778,7 +6777,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A115" s="43">
         <v>114</v>
       </c>
@@ -6792,7 +6791,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A116" s="43">
         <v>115</v>
       </c>
@@ -6806,7 +6805,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A117" s="43">
         <v>116</v>
       </c>
@@ -6820,7 +6819,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A118" s="43">
         <v>117</v>
       </c>
@@ -6828,7 +6827,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A119" s="43">
         <v>118</v>
       </c>
@@ -6836,7 +6835,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A120" s="43">
         <v>119</v>
       </c>
@@ -6844,7 +6843,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A121" s="43">
         <v>120</v>
       </c>
@@ -6852,7 +6851,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A122" s="43">
         <v>121</v>
       </c>
@@ -6860,7 +6859,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A123" s="43">
         <v>122</v>
       </c>
@@ -6868,7 +6867,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A124" s="43">
         <v>123</v>
       </c>
@@ -6882,7 +6881,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A125" s="43">
         <v>124</v>
       </c>
@@ -6896,7 +6895,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A126" s="43">
         <v>125</v>
       </c>
@@ -6910,7 +6909,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A127" s="43">
         <v>126</v>
       </c>
@@ -6918,7 +6917,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A128" s="43">
         <v>127</v>
       </c>
@@ -6926,7 +6925,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A129" s="43">
         <v>128</v>
       </c>
@@ -6934,7 +6933,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A130" s="43">
         <v>129</v>
       </c>
@@ -6948,7 +6947,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A131" s="43">
         <v>130</v>
       </c>
@@ -6962,7 +6961,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A132" s="43">
         <v>131</v>
       </c>
@@ -6976,7 +6975,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A133" s="43">
         <v>132</v>
       </c>
@@ -6984,7 +6983,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A134" s="43">
         <v>133</v>
       </c>
@@ -6992,7 +6991,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A135" s="43">
         <v>134</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A136" s="43">
         <v>135</v>
       </c>
@@ -7008,7 +7007,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A137" s="43">
         <v>136</v>
       </c>
@@ -7019,7 +7018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A138" s="43">
         <v>137</v>
       </c>
@@ -7033,7 +7032,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A139" s="43">
         <v>138</v>
       </c>
@@ -7047,7 +7046,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A140" s="43">
         <v>139</v>
       </c>
@@ -7061,7 +7060,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A141" s="43">
         <v>140</v>
       </c>
@@ -7069,7 +7068,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A142" s="43">
         <v>141</v>
       </c>
@@ -7077,7 +7076,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A143" s="43">
         <v>142</v>
       </c>
@@ -7091,7 +7090,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A144" s="43">
         <v>143</v>
       </c>
@@ -7105,7 +7104,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A145" s="43">
         <v>144</v>
       </c>
@@ -7113,7 +7112,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A146" s="43">
         <v>145</v>
       </c>
@@ -7121,7 +7120,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A147" s="43">
         <v>146</v>
       </c>
@@ -7129,7 +7128,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A148" s="43">
         <v>147</v>
       </c>
@@ -7137,7 +7136,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A149" s="43">
         <v>148</v>
       </c>
@@ -7145,7 +7144,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A150" s="43">
         <v>149</v>
       </c>
@@ -7154,7 +7153,7 @@
       </c>
       <c r="F150" s="43"/>
     </row>
-    <row r="151" spans="1:6" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="87" x14ac:dyDescent="0.4">
       <c r="A151" s="43">
         <v>150</v>
       </c>
@@ -7168,7 +7167,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A152" s="43">
         <v>151</v>
       </c>
@@ -7182,7 +7181,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A153" s="43">
         <v>152</v>
       </c>
@@ -7190,7 +7189,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A154" s="43">
         <v>153</v>
       </c>
@@ -7198,7 +7197,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A155" s="43">
         <v>154</v>
       </c>
@@ -7206,7 +7205,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A156" s="43">
         <v>155</v>
       </c>
@@ -7214,7 +7213,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A157" s="43">
         <v>156</v>
       </c>
@@ -7222,7 +7221,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A158" s="43">
         <v>157</v>
       </c>
@@ -7230,7 +7229,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="264" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="278.39999999999998" x14ac:dyDescent="0.4">
       <c r="A159" s="43">
         <v>158</v>
       </c>
@@ -7244,7 +7243,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A160" s="43">
         <v>159</v>
       </c>
@@ -7252,7 +7251,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A161" s="43">
         <v>160</v>
       </c>
@@ -7260,7 +7259,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A162" s="43">
         <v>161</v>
       </c>
@@ -7268,7 +7267,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A163" s="43">
         <v>162</v>
       </c>
@@ -7277,6 +7276,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B163"/>
   <mergeCells count="1">
     <mergeCell ref="C1:E1"/>
   </mergeCells>
@@ -7287,7 +7287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -7295,12 +7295,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="41" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" style="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="38" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="38" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="40" t="s">
         <v>234</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="41">
         <v>1</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="41">
         <v>2</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="41">
         <v>3</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="41">
         <v>4</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="41">
         <v>5</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="41">
         <v>6</v>
       </c>
@@ -7371,117 +7371,117 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="41">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="41">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="41">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="41">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="41">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="41">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="41">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="41">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="41">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" s="41">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" s="41">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" s="41">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A20" s="41">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A21" s="41">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A22" s="41">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A23" s="41">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A24" s="41">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A25" s="41">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A26" s="41">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A27" s="41">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A28" s="41">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A29" s="41">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A30" s="41">
         <v>29</v>
       </c>
@@ -7493,7 +7493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -7501,13 +7501,13 @@
       <selection activeCell="E9" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.75" style="41" customWidth="1"/>
-    <col min="3" max="3" width="79.875" customWidth="1"/>
+    <col min="1" max="1" width="5.69921875" style="41" customWidth="1"/>
+    <col min="3" max="3" width="79.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="37" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="37" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="40" t="s">
         <v>31</v>
       </c>
@@ -7519,7 +7519,7 @@
       </c>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:4" ht="50.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="52.8" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="41">
         <v>1</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="99" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A3" s="41">
         <v>2</v>
       </c>
@@ -7541,67 +7541,67 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="41">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="41">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="41">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="41">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="41">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="41">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="41">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="41">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="41">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="41">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="41">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="41">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="41">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
StaffDAO수정, StaffDAO Unit Test 하는 중.
</commit_message>
<xml_diff>
--- a/Matrix진행현황관리.xlsx
+++ b/Matrix진행현황관리.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="진행일정" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="437">
   <si>
     <t>업무</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1944,125 +1944,153 @@
   <si>
     <t>팝업 구현 안됨
 수정 기능 구현 안됨
-업무조회 페이지 수정버튼에 연결 안됨</t>
+업무조회 페이지 재배정 기능에 연결 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#서버</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아코디언 구현 되어있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼 구현 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼 구현 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 틀 되어있음
+승인요청/재직/퇴사 각 정보 다름. 수정해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀만 있음
+다시 구현 해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀만 있음.
+다시 구현 해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀만 있음
+다시 구현 해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼 연결 안되어있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀만 있음
+다시 구현 해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀만 있음
+다시 구현해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀만 있음
+다시 구현해야함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구현 끝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs(staff_seq, staff_id, branch_seq, bank_name, account_num, resume_file, health_file, bank_file) values(staff_seq.nextval, ?, ?, ?, ?, ?, ?, ?);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select representative, branch_name, address_city, address_gu, address_dong, address_detail, opening_hour from head_branches where license_num=?;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select count(license_num) from branches where license_num=?;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into admins(admin_seq, admin_id, branch_seq) values(admin_seq.nextval, ?, (select branch_seq from branches where branch_name=?));</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#다시짜야함. 재승인요청or재입사 했을 경우도 같이 출력됨.
+select u.profile_photo, u.name, u.gender, u.birth from users u, staffs s where s.branch_seq=? and s.join_date is not null and s.leave_date is not null And u.user_id=s.staff_id order by u.name asc;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete staffs where staff_id=?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>--전체 직원 목록 보기 
+select u.profile_photo, u.name, u.gender, u.birth, s.work_part from users u, staffs s where s.branch_seq=? And u.user_id=s.staff_id;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>팝업 구현 안됨
 수정 기능 구현 안됨
-업무조회 페이지 재배정 기능에 연결 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구현 됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#서버</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아코디언 구현 되어있음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>버튼 구현 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>버튼 구현 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본 틀 되어있음
-승인요청/재직/퇴사 각 정보 다름. 수정해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀만 있음
-다시 구현 해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀만 있음.
-다시 구현 해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀만 있음
-다시 구현 해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>버튼 연결 안되어있음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀만 있음
-다시 구현 해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀만 있음
-다시 구현해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>틀만 있음
-다시 구현해야함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구현 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구현 끝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DAO 예외처리
-SQL 오류 수정
-DAO 테스트
+업무조회 페이지 수정버튼에 연결 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jUnit-UserDAO 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jUnit-ManualDAO 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무수정 - 팝업 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직원목록 수정
+PPT 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인, 회원가입 정규표현식 추출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL 오류 수정
+ManualDAO, UserDAO 테스트
+예외 발생상황 정리
 UI Event 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into staffs(staff_seq, staff_id, branch_seq, bank_name, account_num, resume_file, health_file, bank_file) values(staff_seq.nextval, ?, ?, ?, ?, ?, ?, ?);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select representative, branch_name, address_city, address_gu, address_dong, address_detail, opening_hour from head_branches where license_num=?;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select count(license_num) from branches where license_num=?;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into admins(admin_seq, admin_id, branch_seq) values(admin_seq.nextval, ?, (select branch_seq from branches where branch_name=?));</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#다시짜야함. 재승인요청or재입사 했을 경우도 같이 출력됨.
-select u.profile_photo, u.name, u.gender, u.birth from users u, staffs s where s.branch_seq=? and s.join_date is not null and s.leave_date is not null And u.user_id=s.staff_id order by u.name asc;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete staffs where staff_id=?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>--전체 직원 목록 보기 
-select u.profile_photo, u.name, u.gender, u.birth, s.work_part from users u, staffs s where s.branch_seq=? And u.user_id=s.staff_id;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지점</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자</t>
+    <t>DailyDAO, StaffDAO 테스트
+예외 발생상황 정리
+DAO 예외처리
+UI Event 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3038,9 +3066,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -3420,14 +3448,31 @@
         <v>43243</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>435</v>
+      </c>
+      <c r="D31" t="s">
+        <v>430</v>
+      </c>
+      <c r="E31" t="s">
+        <v>432</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G31" t="s">
+        <v>431</v>
+      </c>
+      <c r="H31" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="69.599999999999994">
       <c r="B32" s="19">
         <v>43244</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="34" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="B33" s="19">
@@ -3549,9 +3594,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F154" sqref="F154"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -4141,7 +4186,7 @@
         <v>37</v>
       </c>
       <c r="F27" s="117" t="s">
-        <v>404</v>
+        <v>429</v>
       </c>
       <c r="G27" s="29" t="s">
         <v>259</v>
@@ -4427,7 +4472,7 @@
         <v>8</v>
       </c>
       <c r="F41" s="117" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G41" s="29" t="s">
         <v>267</v>
@@ -4569,7 +4614,7 @@
         <v>121</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
@@ -4642,7 +4687,7 @@
         <v>122</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="34.799999999999997">
@@ -4656,7 +4701,7 @@
         <v>123</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>365</v>
@@ -4679,7 +4724,7 @@
         <v>15</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>365</v>
@@ -4702,7 +4747,7 @@
         <v>14</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>365</v>
@@ -4751,7 +4796,7 @@
         <v>17</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>365</v>
@@ -4777,7 +4822,7 @@
         <v>125</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>365</v>
@@ -4803,7 +4848,7 @@
         <v>126</v>
       </c>
       <c r="F57" s="116" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>365</v>
@@ -4829,7 +4874,7 @@
         <v>23</v>
       </c>
       <c r="F58" s="116" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>367</v>
@@ -4896,7 +4941,7 @@
         <v>127</v>
       </c>
       <c r="F63" s="116" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G63" t="s">
         <v>367</v>
@@ -5107,7 +5152,7 @@
         <v>32</v>
       </c>
       <c r="F83" s="116" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -5308,7 +5353,7 @@
         <v>27</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="34.799999999999997">
@@ -5322,7 +5367,7 @@
         <v>28</v>
       </c>
       <c r="F102" s="116" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G102" t="s">
         <v>374</v>
@@ -5390,7 +5435,7 @@
         <v>29</v>
       </c>
       <c r="F106" s="116" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G106" t="s">
         <v>362</v>
@@ -5533,7 +5578,7 @@
         <v>129</v>
       </c>
       <c r="F116" s="116" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -5944,7 +5989,7 @@
         <v>79</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K152" s="8" t="s">
         <v>168</v>
@@ -5964,7 +6009,7 @@
         <v>152</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L153" s="7" t="s">
         <v>153</v>
@@ -6106,7 +6151,7 @@
         <v>150</v>
       </c>
       <c r="G6" s="90" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6117,7 +6162,7 @@
         <v>154</v>
       </c>
       <c r="G7" s="94" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6746,7 +6791,7 @@
       <c r="D56" s="77"/>
       <c r="E56" s="65"/>
       <c r="F56" s="107" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6788,7 +6833,7 @@
         <v>14</v>
       </c>
       <c r="F59" s="52" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6842,7 +6887,7 @@
       </c>
       <c r="E63" s="62"/>
       <c r="F63" s="108" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -7306,7 +7351,7 @@
       <c r="D110" s="87"/>
       <c r="E110" s="88"/>
       <c r="F110" s="89" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -7328,7 +7373,7 @@
       </c>
       <c r="E112" s="93"/>
       <c r="F112" s="94" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -7342,7 +7387,7 @@
       </c>
       <c r="E113" s="113"/>
       <c r="F113" s="114" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="243.6">
@@ -7370,7 +7415,7 @@
       <c r="D115" s="79"/>
       <c r="E115" s="62"/>
       <c r="F115" s="54" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="116" spans="1:6">

</xml_diff>